<commit_message>
8:33 time 26.04.2024 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
@@ -1076,6 +1076,90 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Norqulova Gulhayo Qilich qizi</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>AA7992447</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>066</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Navoiy shahri</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti musiqa rahbari</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>998934314533</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>25-04-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Qarshiboyeva Dildora</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>AB0538735</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>067</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Oqqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>998937022727</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>25-04-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
19:05 time 11.06.2024 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
@@ -4442,6 +4442,636 @@
         </is>
       </c>
     </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Ibadullayeva Ozodaxon Nuraddin qizi</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>AD4790061</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Xiva tumani</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>998914278764</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>15-05-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Rustamova Shohnoza Xushmatovna</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>AB5924952</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>144</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Chilonzor tumani</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>998999319041</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>15-05-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Umarova Feruza Isroiljonovna</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>AD2736984</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>145</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Uchqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>998939422615</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>16-05-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Primqulova Zulfiya Djabbarovna</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>AB2914174</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>146</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Termiz tumani</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>998977940013</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>16-05-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Xasanova maftuna</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>AB1676320</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Andijon tuman</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti defektologi/logopedi</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>998916102810</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>17-05-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Safarova Dildora Shomurotovna</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>AB5494666</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>148</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Termiz tumani</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>998907478616</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>17-05-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Xudoyberdiyeva Barchinoy Sobirovna</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>AA6486701</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Uchqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti musiqa rahbari</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>998947271989</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>20-05-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Karimova Umida Hamroboyevna</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>AA5316053</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Nurota tumani</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>+998934315343</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>20-05-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Allaberganova Sharofat Komiljonovna</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>AD4771702</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Urganch tumani</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>998907192557</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>20-05-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Yuldasheva Zarifaxon Yashinjan qizi</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>AA6363827</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>152</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Andijon tuman</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti defektologi/logopedi</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>+79098312494</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>21-05-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Allayorova Dinora Farhod qizi</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>AB3135777</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Nurota tumani</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti musiqa rahbari</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>+998999573907</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>22-05-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Badalova Dildora Fayzulla qizi</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>AB1866845</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>154</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Mirzo Ulugʻbek tumani</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>998909996877</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>23-05-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Abdullayeva Minajaat Mahkamovna</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>AB6360027</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Uchqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>998937092759</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>27-05-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Sulaymonova Feruza Baxshulloevna</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>AA6765464</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>156</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Navoiy shahri</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti defektologi/logopedi</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>998913308498</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>29-05-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Toxtasinova Munojat Muxammadjon qizi</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>AC0335486</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>157</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Uchqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti musiqa rahbari</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>998933338395</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>05-06-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
8:49 time 20.06.2024 date
</commit_message>
<xml_diff>
--- a/file_service/qabul.xlsx
+++ b/file_service/qabul.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H111"/>
+  <dimension ref="A1:H112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
@@ -5072,6 +5072,48 @@
         </is>
       </c>
     </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Karimova Yulduz Rustam qizi</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>AD5261419</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>158</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Sharof Rashidov tumani</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti psixologi</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>998904888818</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>16-06-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>